<commit_message>
Schedule updated with Assigned Review logs for CDD
</commit_message>
<xml_diff>
--- a/Documents/Second_Week/Project_Schedule_V_2.0.xlsx
+++ b/Documents/Second_Week/Project_Schedule_V_2.0.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\ITI\Embedded Systems\QA_Project\DDM\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\ITI\Embedded Systems\QA_Project\DDM\Documents\Second_Week\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -442,7 +442,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="162">
   <si>
     <t>WBS</t>
   </si>
@@ -1673,6 +1673,49 @@
 10-Ramadan
 11-Yasmine
 12-Mostafa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-Review SRS
+2-Review Test cases
+3-Review Project Plan
+4-Review CM
+5-Review RTM
+6-Review project schedule
+7-CDD DIO
+8- CDD TIM0/TIM2
+9- CDD TIM1
+10-CDD LCD
+11-CDD UltraSonic
+12-CDD RTOS
+13-CDD APP
+14-CDD DIO Review
+15-CDD TIM0/TIM2 Review
+16-CDD TIM1 Review
+17- CDD UltraSonic Review
+18-CDD RTOS Review
+19-CDD APP Review
+</t>
+  </si>
+  <si>
+    <t>1-Mina
+2-Mahmoud
+3-Osama
+4-Omnia
+5-Mahmoud
+6-Omnia/Mostafa
+7-Felo
+8-Esraa ElSaid
+9-Dakak
+10-Ramadan
+11-Yasmine
+12-Mostafa
+13-Mostafa/Esraa
+14-Mostafa
+15-Mostafa
+16-Yasmin
+17-Ramadan
+18-Dakak
+19-Mostafa</t>
   </si>
 </sst>
 </file>
@@ -3066,6 +3109,24 @@
     <xf numFmtId="0" fontId="38" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="41" fillId="27" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="27" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="27" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="72" fillId="27" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="72" fillId="27" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="72" fillId="27" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="64" fillId="26" borderId="0" xfId="34" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -3073,27 +3134,9 @@
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="27" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="27" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="27" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="72" fillId="27" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="167" fontId="72" fillId="27" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="72" fillId="27" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="72" fillId="27" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="52" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -3278,13 +3321,13 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>685800</xdr:colOff>
+      <xdr:colOff>383241</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>123825</xdr:colOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>135031</xdr:colOff>
       <xdr:row>9</xdr:row>
       <xdr:rowOff>70908</xdr:rowOff>
     </xdr:to>
@@ -3929,14 +3972,14 @@
   <dimension ref="A1:BN43"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C21" sqref="C21"/>
+      <pane ySplit="7" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6.85546875" style="3" customWidth="1"/>
-    <col min="2" max="2" width="19" style="1" customWidth="1"/>
+    <col min="2" max="2" width="23.5703125" style="1" customWidth="1"/>
     <col min="3" max="3" width="26.140625" style="1" customWidth="1"/>
     <col min="4" max="4" width="6.85546875" style="4" hidden="1" customWidth="1"/>
     <col min="5" max="6" width="12" style="1" customWidth="1"/>
@@ -3961,29 +4004,29 @@
       <c r="H1" s="157"/>
       <c r="I1" s="158"/>
       <c r="J1" s="157"/>
-      <c r="K1" s="173" t="s">
+      <c r="K1" s="179" t="s">
         <v>151</v>
       </c>
-      <c r="L1" s="173"/>
-      <c r="M1" s="173"/>
-      <c r="N1" s="173"/>
-      <c r="O1" s="173"/>
-      <c r="P1" s="173"/>
-      <c r="Q1" s="173"/>
-      <c r="R1" s="173"/>
-      <c r="S1" s="173"/>
-      <c r="T1" s="173"/>
-      <c r="U1" s="173"/>
-      <c r="V1" s="173"/>
-      <c r="W1" s="173"/>
-      <c r="X1" s="173"/>
-      <c r="Y1" s="173"/>
-      <c r="Z1" s="173"/>
-      <c r="AA1" s="173"/>
-      <c r="AB1" s="173"/>
-      <c r="AC1" s="173"/>
-      <c r="AD1" s="173"/>
-      <c r="AE1" s="173"/>
+      <c r="L1" s="179"/>
+      <c r="M1" s="179"/>
+      <c r="N1" s="179"/>
+      <c r="O1" s="179"/>
+      <c r="P1" s="179"/>
+      <c r="Q1" s="179"/>
+      <c r="R1" s="179"/>
+      <c r="S1" s="179"/>
+      <c r="T1" s="179"/>
+      <c r="U1" s="179"/>
+      <c r="V1" s="179"/>
+      <c r="W1" s="179"/>
+      <c r="X1" s="179"/>
+      <c r="Y1" s="179"/>
+      <c r="Z1" s="179"/>
+      <c r="AA1" s="179"/>
+      <c r="AB1" s="179"/>
+      <c r="AC1" s="179"/>
+      <c r="AD1" s="179"/>
+      <c r="AE1" s="179"/>
       <c r="AF1" s="157"/>
       <c r="AG1" s="157"/>
       <c r="AH1" s="157"/>
@@ -4161,11 +4204,11 @@
       <c r="B4" s="168" t="s">
         <v>76</v>
       </c>
-      <c r="C4" s="178">
+      <c r="C4" s="181">
         <v>43190</v>
       </c>
-      <c r="D4" s="178"/>
-      <c r="E4" s="178"/>
+      <c r="D4" s="181"/>
+      <c r="E4" s="181"/>
       <c r="F4" s="169"/>
       <c r="G4" s="168" t="s">
         <v>75</v>
@@ -4174,182 +4217,182 @@
         <v>1</v>
       </c>
       <c r="J4" s="171"/>
-      <c r="K4" s="175" t="str">
+      <c r="K4" s="173" t="str">
         <f>"Week "&amp;(K6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 1</v>
       </c>
-      <c r="L4" s="176"/>
-      <c r="M4" s="176"/>
-      <c r="N4" s="176"/>
-      <c r="O4" s="176"/>
-      <c r="P4" s="176"/>
-      <c r="Q4" s="177"/>
-      <c r="R4" s="175" t="str">
+      <c r="L4" s="174"/>
+      <c r="M4" s="174"/>
+      <c r="N4" s="174"/>
+      <c r="O4" s="174"/>
+      <c r="P4" s="174"/>
+      <c r="Q4" s="175"/>
+      <c r="R4" s="173" t="str">
         <f>"Week "&amp;(R6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 2</v>
       </c>
-      <c r="S4" s="176"/>
-      <c r="T4" s="176"/>
-      <c r="U4" s="176"/>
-      <c r="V4" s="176"/>
-      <c r="W4" s="176"/>
-      <c r="X4" s="177"/>
-      <c r="Y4" s="175" t="str">
+      <c r="S4" s="174"/>
+      <c r="T4" s="174"/>
+      <c r="U4" s="174"/>
+      <c r="V4" s="174"/>
+      <c r="W4" s="174"/>
+      <c r="X4" s="175"/>
+      <c r="Y4" s="173" t="str">
         <f>"Week "&amp;(Y6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 3</v>
       </c>
-      <c r="Z4" s="176"/>
-      <c r="AA4" s="176"/>
-      <c r="AB4" s="176"/>
-      <c r="AC4" s="176"/>
-      <c r="AD4" s="176"/>
-      <c r="AE4" s="177"/>
-      <c r="AF4" s="175" t="str">
+      <c r="Z4" s="174"/>
+      <c r="AA4" s="174"/>
+      <c r="AB4" s="174"/>
+      <c r="AC4" s="174"/>
+      <c r="AD4" s="174"/>
+      <c r="AE4" s="175"/>
+      <c r="AF4" s="173" t="str">
         <f>"Week "&amp;(AF6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 4</v>
       </c>
-      <c r="AG4" s="176"/>
-      <c r="AH4" s="176"/>
-      <c r="AI4" s="176"/>
-      <c r="AJ4" s="176"/>
-      <c r="AK4" s="176"/>
-      <c r="AL4" s="177"/>
-      <c r="AM4" s="175" t="str">
+      <c r="AG4" s="174"/>
+      <c r="AH4" s="174"/>
+      <c r="AI4" s="174"/>
+      <c r="AJ4" s="174"/>
+      <c r="AK4" s="174"/>
+      <c r="AL4" s="175"/>
+      <c r="AM4" s="173" t="str">
         <f>"Week "&amp;(AM6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 5</v>
       </c>
-      <c r="AN4" s="176"/>
-      <c r="AO4" s="176"/>
-      <c r="AP4" s="176"/>
-      <c r="AQ4" s="176"/>
-      <c r="AR4" s="176"/>
-      <c r="AS4" s="177"/>
-      <c r="AT4" s="175" t="str">
+      <c r="AN4" s="174"/>
+      <c r="AO4" s="174"/>
+      <c r="AP4" s="174"/>
+      <c r="AQ4" s="174"/>
+      <c r="AR4" s="174"/>
+      <c r="AS4" s="175"/>
+      <c r="AT4" s="173" t="str">
         <f>"Week "&amp;(AT6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 6</v>
       </c>
-      <c r="AU4" s="176"/>
-      <c r="AV4" s="176"/>
-      <c r="AW4" s="176"/>
-      <c r="AX4" s="176"/>
-      <c r="AY4" s="176"/>
-      <c r="AZ4" s="177"/>
-      <c r="BA4" s="175" t="str">
+      <c r="AU4" s="174"/>
+      <c r="AV4" s="174"/>
+      <c r="AW4" s="174"/>
+      <c r="AX4" s="174"/>
+      <c r="AY4" s="174"/>
+      <c r="AZ4" s="175"/>
+      <c r="BA4" s="173" t="str">
         <f>"Week "&amp;(BA6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 7</v>
       </c>
-      <c r="BB4" s="176"/>
-      <c r="BC4" s="176"/>
-      <c r="BD4" s="176"/>
-      <c r="BE4" s="176"/>
-      <c r="BF4" s="176"/>
-      <c r="BG4" s="177"/>
-      <c r="BH4" s="175" t="str">
+      <c r="BB4" s="174"/>
+      <c r="BC4" s="174"/>
+      <c r="BD4" s="174"/>
+      <c r="BE4" s="174"/>
+      <c r="BF4" s="174"/>
+      <c r="BG4" s="175"/>
+      <c r="BH4" s="173" t="str">
         <f>"Week "&amp;(BH6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 8</v>
       </c>
-      <c r="BI4" s="176"/>
-      <c r="BJ4" s="176"/>
-      <c r="BK4" s="176"/>
-      <c r="BL4" s="176"/>
-      <c r="BM4" s="176"/>
-      <c r="BN4" s="177"/>
+      <c r="BI4" s="174"/>
+      <c r="BJ4" s="174"/>
+      <c r="BK4" s="174"/>
+      <c r="BL4" s="174"/>
+      <c r="BM4" s="174"/>
+      <c r="BN4" s="175"/>
     </row>
     <row r="5" spans="1:66" s="154" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="167"/>
       <c r="B5" s="168" t="s">
         <v>77</v>
       </c>
-      <c r="C5" s="174" t="s">
+      <c r="C5" s="180" t="s">
         <v>148</v>
       </c>
-      <c r="D5" s="174"/>
-      <c r="E5" s="174"/>
+      <c r="D5" s="180"/>
+      <c r="E5" s="180"/>
       <c r="F5" s="171"/>
       <c r="G5" s="171"/>
       <c r="H5" s="171"/>
       <c r="I5" s="171"/>
       <c r="J5" s="171"/>
-      <c r="K5" s="179">
+      <c r="K5" s="176">
         <f>K6</f>
         <v>43185</v>
       </c>
-      <c r="L5" s="180"/>
-      <c r="M5" s="180"/>
-      <c r="N5" s="180"/>
-      <c r="O5" s="180"/>
-      <c r="P5" s="180"/>
-      <c r="Q5" s="181"/>
-      <c r="R5" s="179">
+      <c r="L5" s="177"/>
+      <c r="M5" s="177"/>
+      <c r="N5" s="177"/>
+      <c r="O5" s="177"/>
+      <c r="P5" s="177"/>
+      <c r="Q5" s="178"/>
+      <c r="R5" s="176">
         <f>R6</f>
         <v>43192</v>
       </c>
-      <c r="S5" s="180"/>
-      <c r="T5" s="180"/>
-      <c r="U5" s="180"/>
-      <c r="V5" s="180"/>
-      <c r="W5" s="180"/>
-      <c r="X5" s="181"/>
-      <c r="Y5" s="179">
+      <c r="S5" s="177"/>
+      <c r="T5" s="177"/>
+      <c r="U5" s="177"/>
+      <c r="V5" s="177"/>
+      <c r="W5" s="177"/>
+      <c r="X5" s="178"/>
+      <c r="Y5" s="176">
         <f>Y6</f>
         <v>43199</v>
       </c>
-      <c r="Z5" s="180"/>
-      <c r="AA5" s="180"/>
-      <c r="AB5" s="180"/>
-      <c r="AC5" s="180"/>
-      <c r="AD5" s="180"/>
-      <c r="AE5" s="181"/>
-      <c r="AF5" s="179">
+      <c r="Z5" s="177"/>
+      <c r="AA5" s="177"/>
+      <c r="AB5" s="177"/>
+      <c r="AC5" s="177"/>
+      <c r="AD5" s="177"/>
+      <c r="AE5" s="178"/>
+      <c r="AF5" s="176">
         <f>AF6</f>
         <v>43206</v>
       </c>
-      <c r="AG5" s="180"/>
-      <c r="AH5" s="180"/>
-      <c r="AI5" s="180"/>
-      <c r="AJ5" s="180"/>
-      <c r="AK5" s="180"/>
-      <c r="AL5" s="181"/>
-      <c r="AM5" s="179">
+      <c r="AG5" s="177"/>
+      <c r="AH5" s="177"/>
+      <c r="AI5" s="177"/>
+      <c r="AJ5" s="177"/>
+      <c r="AK5" s="177"/>
+      <c r="AL5" s="178"/>
+      <c r="AM5" s="176">
         <f>AM6</f>
         <v>43213</v>
       </c>
-      <c r="AN5" s="180"/>
-      <c r="AO5" s="180"/>
-      <c r="AP5" s="180"/>
-      <c r="AQ5" s="180"/>
-      <c r="AR5" s="180"/>
-      <c r="AS5" s="181"/>
-      <c r="AT5" s="179">
+      <c r="AN5" s="177"/>
+      <c r="AO5" s="177"/>
+      <c r="AP5" s="177"/>
+      <c r="AQ5" s="177"/>
+      <c r="AR5" s="177"/>
+      <c r="AS5" s="178"/>
+      <c r="AT5" s="176">
         <f>AT6</f>
         <v>43220</v>
       </c>
-      <c r="AU5" s="180"/>
-      <c r="AV5" s="180"/>
-      <c r="AW5" s="180"/>
-      <c r="AX5" s="180"/>
-      <c r="AY5" s="180"/>
-      <c r="AZ5" s="181"/>
-      <c r="BA5" s="179">
+      <c r="AU5" s="177"/>
+      <c r="AV5" s="177"/>
+      <c r="AW5" s="177"/>
+      <c r="AX5" s="177"/>
+      <c r="AY5" s="177"/>
+      <c r="AZ5" s="178"/>
+      <c r="BA5" s="176">
         <f>BA6</f>
         <v>43227</v>
       </c>
-      <c r="BB5" s="180"/>
-      <c r="BC5" s="180"/>
-      <c r="BD5" s="180"/>
-      <c r="BE5" s="180"/>
-      <c r="BF5" s="180"/>
-      <c r="BG5" s="181"/>
-      <c r="BH5" s="179">
+      <c r="BB5" s="177"/>
+      <c r="BC5" s="177"/>
+      <c r="BD5" s="177"/>
+      <c r="BE5" s="177"/>
+      <c r="BF5" s="177"/>
+      <c r="BG5" s="178"/>
+      <c r="BH5" s="176">
         <f>BH6</f>
         <v>43234</v>
       </c>
-      <c r="BI5" s="180"/>
-      <c r="BJ5" s="180"/>
-      <c r="BK5" s="180"/>
-      <c r="BL5" s="180"/>
-      <c r="BM5" s="180"/>
-      <c r="BN5" s="181"/>
+      <c r="BI5" s="177"/>
+      <c r="BJ5" s="177"/>
+      <c r="BK5" s="177"/>
+      <c r="BL5" s="177"/>
+      <c r="BM5" s="177"/>
+      <c r="BN5" s="178"/>
     </row>
     <row r="6" spans="1:66" s="147" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="148"/>
@@ -6025,15 +6068,15 @@
       <c r="BM21" s="93"/>
       <c r="BN21" s="93"/>
     </row>
-    <row r="22" spans="1:66" s="50" customFormat="1" ht="180" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:66" s="50" customFormat="1" ht="252" x14ac:dyDescent="0.2">
       <c r="A22" s="49">
         <v>2.6</v>
       </c>
       <c r="B22" s="97" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="C22" s="172" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="D22" s="130"/>
       <c r="E22" s="86">
@@ -7774,6 +7817,15 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertRows="0" deleteRows="0"/>
   <mergeCells count="19">
+    <mergeCell ref="K1:AE1"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="R4:X4"/>
+    <mergeCell ref="K4:Q4"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="R5:X5"/>
+    <mergeCell ref="K5:Q5"/>
+    <mergeCell ref="Y4:AE4"/>
+    <mergeCell ref="Y5:AE5"/>
     <mergeCell ref="AF4:AL4"/>
     <mergeCell ref="AF5:AL5"/>
     <mergeCell ref="BH4:BN4"/>
@@ -7784,15 +7836,6 @@
     <mergeCell ref="AM4:AS4"/>
     <mergeCell ref="BA4:BG4"/>
     <mergeCell ref="BA5:BG5"/>
-    <mergeCell ref="K1:AE1"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="R4:X4"/>
-    <mergeCell ref="K4:Q4"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="R5:X5"/>
-    <mergeCell ref="K5:Q5"/>
-    <mergeCell ref="Y4:AE4"/>
-    <mergeCell ref="Y5:AE5"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="H8:H42">

</xml_diff>